<commit_message>
- Added excel file that generates the sql for the initital set of records
</commit_message>
<xml_diff>
--- a/src/test/resources/course-samples.xlsx
+++ b/src/test/resources/course-samples.xlsx
@@ -636,7 +636,7 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+      <selection activeCell="C2" sqref="C2:C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -682,11 +682,11 @@
       </c>
       <c r="E2">
         <f ca="1">INDEX($H$2:$H$4, RANDBETWEEN(1,3))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" t="str">
         <f ca="1">CONCATENATE("INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (",$A2,",'", $B2,"','",$C2,"',",$D2,",",$E2,");")</f>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Curso TDD',15,1);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Curso TDD',15,2);</v>
       </c>
       <c r="G2" t="s">
         <v>33</v>
@@ -701,7 +701,7 @@
       </c>
       <c r="B3" t="str">
         <f t="shared" ref="B3:B50" ca="1" si="0">INDEX($G$2:$G$4, RANDBETWEEN(1,3))</f>
-        <v>Roberto Canales</v>
+        <v>Alberto Moratilla</v>
       </c>
       <c r="C3" t="s">
         <v>31</v>
@@ -711,11 +711,11 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E50" ca="1" si="1">INDEX($H$2:$H$4, RANDBETWEEN(1,3))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F50" ca="1" si="2">CONCATENATE("INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (",$A3,",'", $B3,"','",$C3,"',",$D3,",",$E3,");")</f>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Novedades Java 8',15,1);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Novedades Java 8',15,2);</v>
       </c>
       <c r="G3" t="s">
         <v>34</v>
@@ -730,7 +730,7 @@
       </c>
       <c r="B4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Angel Ruiz</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -740,11 +740,11 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Introducción al lenguaje Java',20,1);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Introducción al lenguaje Java',20,3);</v>
       </c>
       <c r="G4" t="s">
         <v>35</v>
@@ -759,7 +759,7 @@
       </c>
       <c r="B5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Alberto Moratilla</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -769,11 +769,11 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Desarrollo de Aplicaciones Web en Java',20,2);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Desarrollo de Aplicaciones Web en Java',20,1);</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -792,11 +792,11 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Conceptos avanzados de desarrollo Java',20,1);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Conceptos avanzados de desarrollo Java',20,2);</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -805,7 +805,7 @@
       </c>
       <c r="B7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Alberto Moratilla</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -815,11 +815,11 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Arquitectura de Aplicaciones Empresariales Java: JEE',15,2);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Arquitectura de Aplicaciones Empresariales Java: JEE',15,3);</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -828,7 +828,7 @@
       </c>
       <c r="B8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Angel Ruiz</v>
+        <v>Alberto Moratilla</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -842,7 +842,7 @@
       </c>
       <c r="F8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Novedades de Java 7.0',10,3);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Novedades de Java 7.0',10,3);</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -851,7 +851,7 @@
       </c>
       <c r="B9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Roberto Canales</v>
+        <v>Angel Ruiz</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -865,7 +865,7 @@
       </c>
       <c r="F9" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Java y Patrones de Diseño',15,3);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Java y Patrones de Diseño',15,3);</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -897,7 +897,7 @@
       </c>
       <c r="B11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Angel Ruiz</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -907,11 +907,11 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Buenas prácticas en el desarrollo de aplicaciones Java',15,3);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Buenas prácticas en el desarrollo de aplicaciones Java',15,1);</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -930,11 +930,11 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Web Services sobre plataforma Java',20,1);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Web Services sobre plataforma Java',20,2);</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -943,7 +943,7 @@
       </c>
       <c r="B13" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Roberto Canales</v>
+        <v>Angel Ruiz</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -953,11 +953,11 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Seguridad en Java',25,1);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Seguridad en Java',25,3);</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -976,11 +976,11 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Construcción de aplicaciones con Maven',10,3);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Construcción de aplicaciones con Maven',10,1);</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -989,7 +989,7 @@
       </c>
       <c r="B15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Roberto Canales</v>
+        <v>Alberto Moratilla</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
@@ -999,11 +999,11 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (false,'Roberto Canales','Control de versiones con SubVersion/CVS',15,1);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (false,'Alberto Moratilla','Control de versiones con SubVersion/CVS',15,3);</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1012,7 +1012,7 @@
       </c>
       <c r="B16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Angel Ruiz</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
@@ -1026,7 +1026,7 @@
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Generación de informes con JasperReports/iReport',15,1);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Generación de informes con JasperReports/iReport',15,1);</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1035,7 +1035,7 @@
       </c>
       <c r="B17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Angel Ruiz</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
@@ -1045,11 +1045,11 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Integración de plataformas con arquitecturas ESB: Mule',20,1);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Integración de plataformas con arquitecturas ESB: Mule',20,3);</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1068,11 +1068,11 @@
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Arquitecturas Orientadas a Servicios: SOA',15,1);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Arquitecturas Orientadas a Servicios: SOA',15,3);</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1081,7 +1081,7 @@
       </c>
       <c r="B19" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Alberto Moratilla</v>
+        <v>Angel Ruiz</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -1091,11 +1091,11 @@
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Desarrollo de aplicaciones Ajax',15,2);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Desarrollo de aplicaciones Ajax',15,1);</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1104,7 +1104,7 @@
       </c>
       <c r="B20" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Roberto Canales</v>
+        <v>Alberto Moratilla</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
@@ -1114,11 +1114,11 @@
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Desarrollo de aplicaciones Web con Spring',15,2);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Desarrollo de aplicaciones Web con Spring',15,1);</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="B21" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Angel Ruiz</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
@@ -1141,7 +1141,7 @@
       </c>
       <c r="F21" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (false,'Angel Ruiz','Introducción a JSF',15,1);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (false,'Roberto Canales','Introducción a JSF',15,1);</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1150,7 +1150,7 @@
       </c>
       <c r="B22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Alberto Moratilla</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C22" t="s">
         <v>19</v>
@@ -1160,11 +1160,11 @@
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (false,'Alberto Moratilla','Introducción a Struts',15,3);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (false,'Roberto Canales','Introducción a Struts',15,2);</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1173,7 +1173,7 @@
       </c>
       <c r="B23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Angel Ruiz</v>
+        <v>Alberto Moratilla</v>
       </c>
       <c r="C23" t="s">
         <v>20</v>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="F23" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Acceso a datos con Hibernate',15,2);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Acceso a datos con Hibernate',15,2);</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1206,11 +1206,11 @@
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (false,'Roberto Canales','Acceso a datos con MyBatis',15,1);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (false,'Roberto Canales','Acceso a datos con MyBatis',15,2);</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1219,7 +1219,7 @@
       </c>
       <c r="B25" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Alberto Moratilla</v>
+        <v>Angel Ruiz</v>
       </c>
       <c r="C25" t="s">
         <v>27</v>
@@ -1229,11 +1229,11 @@
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','El motor de bœsqueda Solr',25,1);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','El motor de bœsqueda Solr',25,3);</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1242,7 +1242,7 @@
       </c>
       <c r="B26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Alberto Moratilla</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C26" t="s">
         <v>22</v>
@@ -1252,11 +1252,11 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Maven + Spring + Hibernate + EJB',25,3);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Maven + Spring + Hibernate + EJB',25,2);</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1265,7 +1265,7 @@
       </c>
       <c r="B27" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Roberto Canales</v>
+        <v>Angel Ruiz</v>
       </c>
       <c r="C27" t="s">
         <v>23</v>
@@ -1279,7 +1279,7 @@
       </c>
       <c r="F27" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (false,'Roberto Canales','Maven + JSF + Ajax + Facelets + EJB 3.0',20,2);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (false,'Angel Ruiz','Maven + JSF + Ajax + Facelets + EJB 3.0',20,2);</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="B28" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Angel Ruiz</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C28" t="s">
         <v>24</v>
@@ -1298,11 +1298,11 @@
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Administración y despliegue de aplicaciones con JBoss',15,3);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Administración y despliegue de aplicaciones con JBoss',15,2);</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1311,7 +1311,7 @@
       </c>
       <c r="B29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Angel Ruiz</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C29" t="s">
         <v>25</v>
@@ -1321,11 +1321,11 @@
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Fundamentos de Scala',20,3);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Fundamentos de Scala',20,1);</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1344,11 +1344,11 @@
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Pruebas de aceptación para aplicaciones Web',20,3);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Pruebas de aceptación para aplicaciones Web',20,2);</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1380,7 +1380,7 @@
       </c>
       <c r="B32" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Angel Ruiz</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C32" t="s">
         <v>42</v>
@@ -1390,11 +1390,11 @@
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Dirección de Proyectos y Gestión Eficiente de Equipos',15,3);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Dirección de Proyectos y Gestión Eficiente de Equipos',15,2);</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1426,7 +1426,7 @@
       </c>
       <c r="B34" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Angel Ruiz</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C34" t="s">
         <v>44</v>
@@ -1436,11 +1436,11 @@
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Gestión eficaz del tiempo y eficacia personal',25,1);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Gestión eficaz del tiempo y eficacia personal',25,2);</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="B35" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Alberto Moratilla</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C35" t="s">
         <v>45</v>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="F35" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Metodologías Ágiles: Scrum, Kanban',25,1);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Metodologías Ágiles: Scrum, Kanban',25,1);</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1472,7 +1472,7 @@
       </c>
       <c r="B36" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Alberto Moratilla</v>
+        <v>Angel Ruiz</v>
       </c>
       <c r="C36" t="s">
         <v>46</v>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="F36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Introducción a las nuevas tecnologías',15,3);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Introducción a las nuevas tecnologías',15,3);</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1495,7 +1495,7 @@
       </c>
       <c r="B37" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Alberto Moratilla</v>
+        <v>Angel Ruiz</v>
       </c>
       <c r="C37" t="s">
         <v>39</v>
@@ -1505,11 +1505,11 @@
       </c>
       <c r="E37">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Introducción a la Orientación a Objetos',15,2);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Introducción a la Orientación a Objetos',15,1);</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1518,7 +1518,7 @@
       </c>
       <c r="B38" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Roberto Canales</v>
+        <v>Angel Ruiz</v>
       </c>
       <c r="C38" t="s">
         <v>40</v>
@@ -1528,11 +1528,11 @@
       </c>
       <c r="E38">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Análisis y diseño orientado a objetos con UML 2.x',25,3);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Análisis y diseño orientado a objetos con UML 2.x',25,1);</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1551,11 +1551,11 @@
       </c>
       <c r="E39">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Accesibilidad Web',10,3);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Accesibilidad Web',10,2);</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1564,7 +1564,7 @@
       </c>
       <c r="B40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Alberto Moratilla</v>
+        <v>Angel Ruiz</v>
       </c>
       <c r="C40" t="s">
         <v>48</v>
@@ -1578,7 +1578,7 @@
       </c>
       <c r="F40" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Desarrollo de páginas Web: HTML 5, CSS 3, JavaScript',10,2);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Desarrollo de páginas Web: HTML 5, CSS 3, JavaScript',10,2);</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1587,7 +1587,7 @@
       </c>
       <c r="B41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Angel Ruiz</v>
+        <v>Alberto Moratilla</v>
       </c>
       <c r="C41" t="s">
         <v>49</v>
@@ -1601,7 +1601,7 @@
       </c>
       <c r="F41" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Introducción a la Gestión de Contenidos',15,2);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Introducción a la Gestión de Contenidos',15,2);</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1610,7 +1610,7 @@
       </c>
       <c r="B42" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Angel Ruiz</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C42" t="s">
         <v>50</v>
@@ -1620,11 +1620,11 @@
       </c>
       <c r="E42">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Desarrollo de aplicaciones con Liferay',20,2);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Desarrollo de aplicaciones con Liferay',20,3);</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1633,7 +1633,7 @@
       </c>
       <c r="B43" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Alberto Moratilla</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C43" t="s">
         <v>51</v>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="F43" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Administración de Liferay',20,2);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Administración de Liferay',20,2);</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1656,7 +1656,7 @@
       </c>
       <c r="B44" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Angel Ruiz</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C44" t="s">
         <v>52</v>
@@ -1666,11 +1666,11 @@
       </c>
       <c r="E44">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Desarrollo de aplicaciones con Alfresco',25,1);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Desarrollo de aplicaciones con Alfresco',25,2);</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1679,7 +1679,7 @@
       </c>
       <c r="B45" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Alberto Moratilla</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C45" t="s">
         <v>53</v>
@@ -1689,11 +1689,11 @@
       </c>
       <c r="E45">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Administración de Alfresco',20,3);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Administración de Alfresco',20,2);</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1702,7 +1702,7 @@
       </c>
       <c r="B46" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Alberto Moratilla</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C46" t="s">
         <v>54</v>
@@ -1716,7 +1716,7 @@
       </c>
       <c r="F46" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Programación de aplicaciones sobre iPhone',10,1);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Programación de aplicaciones sobre iPhone',10,1);</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1725,7 +1725,7 @@
       </c>
       <c r="B47" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Alberto Moratilla</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C47" t="s">
         <v>55</v>
@@ -1739,7 +1739,7 @@
       </c>
       <c r="F47" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Programación de aplicaciones sobre Android',10,3);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Programación de aplicaciones sobre Android',10,3);</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1748,7 +1748,7 @@
       </c>
       <c r="B48" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Alberto Moratilla</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C48" t="s">
         <v>56</v>
@@ -1758,11 +1758,11 @@
       </c>
       <c r="E48">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Alberto Moratilla','Desarrollo de aplicaciones con C/C++',15,3);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Desarrollo de aplicaciones con C/C++',15,2);</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1781,11 +1781,11 @@
       </c>
       <c r="E49">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Introducción a MySQL',15,2);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Introducción a MySQL',15,3);</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1794,7 +1794,7 @@
       </c>
       <c r="B50" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Angel Ruiz</v>
+        <v>Roberto Canales</v>
       </c>
       <c r="C50" t="s">
         <v>58</v>
@@ -1804,11 +1804,11 @@
       </c>
       <c r="E50">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F50" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Angel Ruiz','Introducción a Linux',15,3);</v>
+        <v>INSERT INTO TRAINING.course (active,teacher,title,hours,level) VALUES (true,'Roberto Canales','Introducción a Linux',15,1);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>